<commit_message>
Natalia Bernal, creación de dasboard
</commit_message>
<xml_diff>
--- a/DATABANK/Content/uploads/Plantilla.xlsx
+++ b/DATABANK/Content/uploads/Plantilla.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>BODEGA</t>
   </si>
@@ -65,9 +65,6 @@
     <t>DESCRIPCION</t>
   </si>
   <si>
-    <t>BODEGA SEGUNDARIA</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -95,7 +92,19 @@
     <t>BAQLDE</t>
   </si>
   <si>
-    <t xml:space="preserve">BODEGA </t>
+    <t>Bodega 1</t>
+  </si>
+  <si>
+    <t>Bodega 2</t>
+  </si>
+  <si>
+    <t>Bodega 3</t>
+  </si>
+  <si>
+    <t>Bodega 4</t>
+  </si>
+  <si>
+    <t>Bodega 5</t>
   </si>
 </sst>
 </file>
@@ -433,7 +442,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C18" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,19 +504,19 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
       </c>
       <c r="H2">
         <v>20</v>
@@ -530,19 +539,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>30</v>
@@ -554,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -565,19 +574,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4">
         <v>40</v>
@@ -600,19 +609,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5">
         <v>50</v>
@@ -635,19 +644,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6">
         <v>60</v>

</xml_diff>